<commit_message>
add how doubles are managed
</commit_message>
<xml_diff>
--- a/match_details.xlsx
+++ b/match_details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\capna\Downloads\rsc_speedball\Scoreboard generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8297FEA-6547-4567-81EF-C356643ADE4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209A4FE7-467D-416C-8F95-D40531EC8D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30735" yWindow="0" windowWidth="21570" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="match_details" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>date</t>
   </si>
@@ -55,34 +55,60 @@
     <t>club_2</t>
   </si>
   <si>
-    <t>Cairo International Stadium</t>
+    <t>Men</t>
   </si>
   <si>
-    <t>QF</t>
+    <t>write the month first when changing date entry [mm-dd-yyyy]</t>
+  </si>
+  <si>
+    <t>U-15</t>
+  </si>
+  <si>
+    <t>R2</t>
   </si>
   <si>
     <t>Doubles</t>
   </si>
   <si>
-    <t>Women</t>
+    <t>Ipsum Lorem &amp; Lorem Ipsum</t>
   </si>
   <si>
-    <t>Zohour-ZSC</t>
+    <t>Lorem Ipsum &amp; Ipsum Lorem</t>
   </si>
   <si>
-    <t>Heliopolis-HSC</t>
+    <t>Final</t>
   </si>
   <si>
-    <t>Seniors</t>
+    <t>for player_1 &amp; player_2: if event is singles [format: Lorem Ipsum] else if event is doubles [format: Lorem Ipsum &amp; Ipsum Lorem]</t>
   </si>
   <si>
-    <t>Nader Safa</t>
+    <t>Suez Canal-SSC</t>
   </si>
   <si>
-    <t>Omar Nagah</t>
+    <t>Cairo International Stadium</t>
   </si>
   <si>
-    <t>National</t>
+    <r>
+      <t xml:space="preserve">DO NOT EDIT </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="22"/>
+        <color rgb="FF2ED573"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">GREEN </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="22"/>
+        <color rgb="FFF4F4F4"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>CELLS</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -92,7 +118,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,8 +253,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF171717"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color rgb="FFF4F4F4"/>
+      <name val="Montserrat"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color rgb="FF2ED573"/>
+      <name val="Montserrat"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -406,6 +451,24 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2ED573"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4F4F4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF4757"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -569,10 +632,35 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="18" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -620,6 +708,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF2ED573"/>
+      <color rgb="FFFF4757"/>
+      <color rgb="FFF4F4F4"/>
+      <color rgb="FF171717"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -931,2163 +1027,2115 @@
   <dimension ref="A1:K483"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="118" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D2" sqref="D2:K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" style="2" customWidth="1"/>
+    <col min="2" max="3" width="25.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.21875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="11.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+      <c r="A2" s="3">
         <v>44653</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="H2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B3" s="2">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="5">
         <v>0</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C5" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="2">
+      <c r="D5" s="1"/>
+      <c r="F5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="5">
         <v>0</v>
       </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="2">
+      <c r="C6" s="5">
         <v>0</v>
       </c>
-      <c r="C5" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="2">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2">
-        <v>2</v>
-      </c>
+      <c r="D6" s="1"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="2">
-        <v>2</v>
-      </c>
-      <c r="C7" s="2">
-        <v>2</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B8" s="2">
-        <v>3</v>
-      </c>
-      <c r="C8" s="2">
-        <v>2</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="5">
+        <v>0</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B9" s="2">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2">
-        <v>3</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="5">
+        <v>0</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B10" s="2">
-        <v>4</v>
-      </c>
-      <c r="C10" s="2">
-        <v>3</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="5">
+        <v>0</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="2">
-        <v>4</v>
-      </c>
-      <c r="C11" s="2">
-        <v>4</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="5">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="2">
-        <v>5</v>
-      </c>
-      <c r="C12" s="2">
-        <v>4</v>
+      <c r="B12" s="5">
+        <v>0</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="2">
-        <v>5</v>
-      </c>
-      <c r="C13" s="2">
-        <v>5</v>
-      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="2">
-        <v>6</v>
-      </c>
-      <c r="C14" s="2">
-        <v>5</v>
-      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="2">
-        <v>7</v>
-      </c>
-      <c r="C15" s="2">
-        <v>5</v>
-      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="2">
-        <v>7</v>
-      </c>
-      <c r="C16" s="2">
-        <v>6</v>
-      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="2">
-        <v>7</v>
-      </c>
-      <c r="C17" s="2">
-        <v>7</v>
-      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="2">
-        <v>8</v>
-      </c>
-      <c r="C18" s="2">
-        <v>7</v>
-      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19" s="2">
-        <v>8</v>
-      </c>
-      <c r="C19" s="2">
-        <v>8</v>
-      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B20" s="2">
-        <v>9</v>
-      </c>
-      <c r="C20" s="2">
-        <v>8</v>
-      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B21" s="2">
-        <v>10</v>
-      </c>
-      <c r="C21" s="2">
-        <v>8</v>
-      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B22" s="2">
-        <v>0</v>
-      </c>
-      <c r="C22" s="2">
-        <v>0</v>
-      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B23" s="2">
-        <v>1</v>
-      </c>
-      <c r="C23" s="2">
-        <v>0</v>
-      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B24" s="2">
-        <v>2</v>
-      </c>
-      <c r="C24" s="2">
-        <v>0</v>
-      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B25" s="2">
-        <v>3</v>
-      </c>
-      <c r="C25" s="2">
-        <v>0</v>
-      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B26" s="2">
-        <v>4</v>
-      </c>
-      <c r="C26" s="2">
-        <v>0</v>
-      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B27" s="2">
-        <v>4</v>
-      </c>
-      <c r="C27" s="2">
-        <v>1</v>
-      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B28" s="2">
-        <v>4</v>
-      </c>
-      <c r="C28" s="2">
-        <v>2</v>
-      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B29" s="2">
-        <v>5</v>
-      </c>
-      <c r="C29" s="2">
-        <v>2</v>
-      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B30" s="2">
-        <v>6</v>
-      </c>
-      <c r="C30" s="2">
-        <v>2</v>
-      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B31" s="2">
-        <v>6</v>
-      </c>
-      <c r="C31" s="2">
-        <v>3</v>
-      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B32" s="2">
-        <v>7</v>
-      </c>
-      <c r="C32" s="2">
-        <v>3</v>
-      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B33" s="2">
-        <v>8</v>
-      </c>
-      <c r="C33" s="2">
-        <v>3</v>
-      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B34" s="2">
-        <v>8</v>
-      </c>
-      <c r="C34" s="2">
-        <v>4</v>
-      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B35" s="2">
-        <v>9</v>
-      </c>
-      <c r="C35" s="2">
-        <v>4</v>
-      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B36" s="2">
-        <v>9</v>
-      </c>
-      <c r="C36" s="2">
-        <v>5</v>
-      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B37" s="2">
-        <v>10</v>
-      </c>
-      <c r="C37" s="2">
-        <v>5</v>
-      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B38" s="2">
-        <v>0</v>
-      </c>
-      <c r="C38" s="2">
-        <v>0</v>
-      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B74" s="2"/>
-      <c r="C74" s="2"/>
+      <c r="B74" s="5"/>
+      <c r="C74" s="5"/>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
+      <c r="B76" s="5"/>
+      <c r="C76" s="5"/>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B77" s="2"/>
-      <c r="C77" s="2"/>
+      <c r="B77" s="5"/>
+      <c r="C77" s="5"/>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B78" s="2"/>
-      <c r="C78" s="2"/>
+      <c r="B78" s="5"/>
+      <c r="C78" s="5"/>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B79" s="2"/>
-      <c r="C79" s="2"/>
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
+      <c r="B80" s="5"/>
+      <c r="C80" s="5"/>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
+      <c r="B81" s="5"/>
+      <c r="C81" s="5"/>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B82" s="2"/>
-      <c r="C82" s="2"/>
+      <c r="B82" s="5"/>
+      <c r="C82" s="5"/>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
+      <c r="B83" s="5"/>
+      <c r="C83" s="5"/>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B84" s="2"/>
-      <c r="C84" s="2"/>
+      <c r="B84" s="5"/>
+      <c r="C84" s="5"/>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B85" s="2"/>
-      <c r="C85" s="2"/>
+      <c r="B85" s="5"/>
+      <c r="C85" s="5"/>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B86" s="2"/>
-      <c r="C86" s="2"/>
+      <c r="B86" s="5"/>
+      <c r="C86" s="5"/>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B87" s="2"/>
-      <c r="C87" s="2"/>
+      <c r="B87" s="5"/>
+      <c r="C87" s="5"/>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B88" s="2"/>
-      <c r="C88" s="2"/>
+      <c r="B88" s="5"/>
+      <c r="C88" s="5"/>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B89" s="2"/>
-      <c r="C89" s="2"/>
+      <c r="B89" s="5"/>
+      <c r="C89" s="5"/>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B90" s="2"/>
-      <c r="C90" s="2"/>
+      <c r="B90" s="5"/>
+      <c r="C90" s="5"/>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B91" s="2"/>
-      <c r="C91" s="2"/>
+      <c r="B91" s="5"/>
+      <c r="C91" s="5"/>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B92" s="2"/>
-      <c r="C92" s="2"/>
+      <c r="B92" s="5"/>
+      <c r="C92" s="5"/>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B93" s="2"/>
-      <c r="C93" s="2"/>
+      <c r="B93" s="5"/>
+      <c r="C93" s="5"/>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B94" s="2"/>
-      <c r="C94" s="2"/>
+      <c r="B94" s="5"/>
+      <c r="C94" s="5"/>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B95" s="2"/>
-      <c r="C95" s="2"/>
+      <c r="B95" s="5"/>
+      <c r="C95" s="5"/>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B96" s="2"/>
-      <c r="C96" s="2"/>
+      <c r="B96" s="5"/>
+      <c r="C96" s="5"/>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B97" s="2"/>
-      <c r="C97" s="2"/>
+      <c r="B97" s="5"/>
+      <c r="C97" s="5"/>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B98" s="2"/>
-      <c r="C98" s="2"/>
+      <c r="B98" s="5"/>
+      <c r="C98" s="5"/>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B99" s="2"/>
-      <c r="C99" s="2"/>
+      <c r="B99" s="5"/>
+      <c r="C99" s="5"/>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B100" s="2"/>
-      <c r="C100" s="2"/>
+      <c r="B100" s="5"/>
+      <c r="C100" s="5"/>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B101" s="2"/>
-      <c r="C101" s="2"/>
+      <c r="B101" s="6"/>
+      <c r="C101" s="6"/>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B102" s="2"/>
-      <c r="C102" s="2"/>
+      <c r="B102" s="6"/>
+      <c r="C102" s="6"/>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B103" s="2"/>
-      <c r="C103" s="2"/>
+      <c r="B103" s="6"/>
+      <c r="C103" s="6"/>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B104" s="2"/>
-      <c r="C104" s="2"/>
+      <c r="B104" s="6"/>
+      <c r="C104" s="6"/>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B105" s="2"/>
-      <c r="C105" s="2"/>
+      <c r="B105" s="6"/>
+      <c r="C105" s="6"/>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B106" s="2"/>
-      <c r="C106" s="2"/>
+      <c r="B106" s="6"/>
+      <c r="C106" s="6"/>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B107" s="2"/>
-      <c r="C107" s="2"/>
+      <c r="B107" s="6"/>
+      <c r="C107" s="6"/>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B108" s="2"/>
-      <c r="C108" s="2"/>
+      <c r="B108" s="6"/>
+      <c r="C108" s="6"/>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B109" s="2"/>
-      <c r="C109" s="2"/>
+      <c r="B109" s="6"/>
+      <c r="C109" s="6"/>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B110" s="2"/>
-      <c r="C110" s="2"/>
+      <c r="B110" s="6"/>
+      <c r="C110" s="6"/>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B111" s="2"/>
-      <c r="C111" s="2"/>
+      <c r="B111" s="6"/>
+      <c r="C111" s="6"/>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B112" s="2"/>
-      <c r="C112" s="2"/>
+      <c r="B112" s="6"/>
+      <c r="C112" s="6"/>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B113" s="2"/>
-      <c r="C113" s="2"/>
+      <c r="B113" s="6"/>
+      <c r="C113" s="6"/>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B114" s="2"/>
-      <c r="C114" s="2"/>
+      <c r="B114" s="6"/>
+      <c r="C114" s="6"/>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B115" s="2"/>
-      <c r="C115" s="2"/>
+      <c r="B115" s="6"/>
+      <c r="C115" s="6"/>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B116" s="2"/>
-      <c r="C116" s="2"/>
+      <c r="B116" s="6"/>
+      <c r="C116" s="6"/>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B117" s="2"/>
-      <c r="C117" s="2"/>
+      <c r="B117" s="6"/>
+      <c r="C117" s="6"/>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B118" s="2"/>
-      <c r="C118" s="2"/>
+      <c r="B118" s="6"/>
+      <c r="C118" s="6"/>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B119" s="2"/>
-      <c r="C119" s="2"/>
+      <c r="B119" s="6"/>
+      <c r="C119" s="6"/>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B120" s="2"/>
-      <c r="C120" s="2"/>
+      <c r="B120" s="6"/>
+      <c r="C120" s="6"/>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B121" s="2"/>
-      <c r="C121" s="2"/>
+      <c r="B121" s="6"/>
+      <c r="C121" s="6"/>
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B122" s="2"/>
-      <c r="C122" s="2"/>
+      <c r="B122" s="6"/>
+      <c r="C122" s="6"/>
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B123" s="2"/>
-      <c r="C123" s="2"/>
+      <c r="B123" s="6"/>
+      <c r="C123" s="6"/>
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B124" s="2"/>
-      <c r="C124" s="2"/>
+      <c r="B124" s="6"/>
+      <c r="C124" s="6"/>
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B125" s="2"/>
-      <c r="C125" s="2"/>
+      <c r="B125" s="6"/>
+      <c r="C125" s="6"/>
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B126" s="2"/>
-      <c r="C126" s="2"/>
+      <c r="B126" s="6"/>
+      <c r="C126" s="6"/>
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B127" s="2"/>
-      <c r="C127" s="2"/>
+      <c r="B127" s="6"/>
+      <c r="C127" s="6"/>
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B128" s="2"/>
-      <c r="C128" s="2"/>
+      <c r="B128" s="6"/>
+      <c r="C128" s="6"/>
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B129" s="2"/>
-      <c r="C129" s="2"/>
+      <c r="B129" s="6"/>
+      <c r="C129" s="6"/>
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B130" s="2"/>
-      <c r="C130" s="2"/>
+      <c r="B130" s="6"/>
+      <c r="C130" s="6"/>
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B131" s="2"/>
-      <c r="C131" s="2"/>
+      <c r="B131" s="6"/>
+      <c r="C131" s="6"/>
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B132" s="2"/>
-      <c r="C132" s="2"/>
+      <c r="B132" s="6"/>
+      <c r="C132" s="6"/>
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B133" s="2"/>
-      <c r="C133" s="2"/>
+      <c r="B133" s="6"/>
+      <c r="C133" s="6"/>
     </row>
     <row r="134" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B134" s="2"/>
-      <c r="C134" s="2"/>
+      <c r="B134" s="6"/>
+      <c r="C134" s="6"/>
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B135" s="2"/>
-      <c r="C135" s="2"/>
+      <c r="B135" s="6"/>
+      <c r="C135" s="6"/>
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B136" s="2"/>
-      <c r="C136" s="2"/>
+      <c r="B136" s="6"/>
+      <c r="C136" s="6"/>
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B137" s="2"/>
-      <c r="C137" s="2"/>
+      <c r="B137" s="6"/>
+      <c r="C137" s="6"/>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B138" s="2"/>
-      <c r="C138" s="2"/>
+      <c r="B138" s="6"/>
+      <c r="C138" s="6"/>
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B139" s="2"/>
-      <c r="C139" s="2"/>
+      <c r="B139" s="6"/>
+      <c r="C139" s="6"/>
     </row>
     <row r="140" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B140" s="2"/>
-      <c r="C140" s="2"/>
+      <c r="B140" s="6"/>
+      <c r="C140" s="6"/>
     </row>
     <row r="141" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B141" s="2"/>
-      <c r="C141" s="2"/>
+      <c r="B141" s="6"/>
+      <c r="C141" s="6"/>
     </row>
     <row r="142" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B142" s="2"/>
-      <c r="C142" s="2"/>
+      <c r="B142" s="6"/>
+      <c r="C142" s="6"/>
     </row>
     <row r="143" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B143" s="2"/>
-      <c r="C143" s="2"/>
+      <c r="B143" s="6"/>
+      <c r="C143" s="6"/>
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B144" s="2"/>
-      <c r="C144" s="2"/>
+      <c r="B144" s="6"/>
+      <c r="C144" s="6"/>
     </row>
     <row r="145" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B145" s="2"/>
-      <c r="C145" s="2"/>
+      <c r="B145" s="6"/>
+      <c r="C145" s="6"/>
     </row>
     <row r="146" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B146" s="2"/>
-      <c r="C146" s="2"/>
+      <c r="B146" s="6"/>
+      <c r="C146" s="6"/>
     </row>
     <row r="147" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B147" s="2"/>
-      <c r="C147" s="2"/>
+      <c r="B147" s="6"/>
+      <c r="C147" s="6"/>
     </row>
     <row r="148" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B148" s="2"/>
-      <c r="C148" s="2"/>
+      <c r="B148" s="6"/>
+      <c r="C148" s="6"/>
     </row>
     <row r="149" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B149" s="2"/>
-      <c r="C149" s="2"/>
+      <c r="B149" s="6"/>
+      <c r="C149" s="6"/>
     </row>
     <row r="150" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B150" s="2"/>
-      <c r="C150" s="2"/>
+      <c r="B150" s="6"/>
+      <c r="C150" s="6"/>
     </row>
     <row r="151" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B151" s="2"/>
-      <c r="C151" s="2"/>
+      <c r="B151" s="6"/>
+      <c r="C151" s="6"/>
     </row>
     <row r="152" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B152" s="2"/>
-      <c r="C152" s="2"/>
+      <c r="B152" s="6"/>
+      <c r="C152" s="6"/>
     </row>
     <row r="153" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B153" s="2"/>
-      <c r="C153" s="2"/>
+      <c r="B153" s="6"/>
+      <c r="C153" s="6"/>
     </row>
     <row r="154" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B154" s="2"/>
-      <c r="C154" s="2"/>
+      <c r="B154" s="6"/>
+      <c r="C154" s="6"/>
     </row>
     <row r="155" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B155" s="2"/>
-      <c r="C155" s="2"/>
+      <c r="B155" s="6"/>
+      <c r="C155" s="6"/>
     </row>
     <row r="156" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B156" s="2"/>
-      <c r="C156" s="2"/>
+      <c r="B156" s="6"/>
+      <c r="C156" s="6"/>
     </row>
     <row r="157" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B157" s="2"/>
-      <c r="C157" s="2"/>
+      <c r="B157" s="6"/>
+      <c r="C157" s="6"/>
     </row>
     <row r="158" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B158" s="2"/>
-      <c r="C158" s="2"/>
+      <c r="B158" s="6"/>
+      <c r="C158" s="6"/>
     </row>
     <row r="159" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B159" s="2"/>
-      <c r="C159" s="2"/>
+      <c r="B159" s="6"/>
+      <c r="C159" s="6"/>
     </row>
     <row r="160" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B160" s="2"/>
-      <c r="C160" s="2"/>
+      <c r="B160" s="6"/>
+      <c r="C160" s="6"/>
     </row>
     <row r="161" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B161" s="2"/>
-      <c r="C161" s="2"/>
+      <c r="B161" s="6"/>
+      <c r="C161" s="6"/>
     </row>
     <row r="162" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B162" s="2"/>
-      <c r="C162" s="2"/>
+      <c r="B162" s="6"/>
+      <c r="C162" s="6"/>
     </row>
     <row r="163" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B163" s="2"/>
-      <c r="C163" s="2"/>
+      <c r="B163" s="6"/>
+      <c r="C163" s="6"/>
     </row>
     <row r="164" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B164" s="2"/>
-      <c r="C164" s="2"/>
+      <c r="B164" s="6"/>
+      <c r="C164" s="6"/>
     </row>
     <row r="165" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B165" s="2"/>
-      <c r="C165" s="2"/>
+      <c r="B165" s="6"/>
+      <c r="C165" s="6"/>
     </row>
     <row r="166" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B166" s="2"/>
-      <c r="C166" s="2"/>
+      <c r="B166" s="6"/>
+      <c r="C166" s="6"/>
     </row>
     <row r="167" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B167" s="2"/>
-      <c r="C167" s="2"/>
+      <c r="B167" s="6"/>
+      <c r="C167" s="6"/>
     </row>
     <row r="168" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B168" s="2"/>
-      <c r="C168" s="2"/>
+      <c r="B168" s="6"/>
+      <c r="C168" s="6"/>
     </row>
     <row r="169" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B169" s="2"/>
-      <c r="C169" s="2"/>
+      <c r="B169" s="6"/>
+      <c r="C169" s="6"/>
     </row>
     <row r="170" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B170" s="2"/>
-      <c r="C170" s="2"/>
+      <c r="B170" s="6"/>
+      <c r="C170" s="6"/>
     </row>
     <row r="171" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B171" s="2"/>
-      <c r="C171" s="2"/>
+      <c r="B171" s="6"/>
+      <c r="C171" s="6"/>
     </row>
     <row r="172" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B172" s="2"/>
-      <c r="C172" s="2"/>
+      <c r="B172" s="6"/>
+      <c r="C172" s="6"/>
     </row>
     <row r="173" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B173" s="2"/>
-      <c r="C173" s="2"/>
+      <c r="B173" s="6"/>
+      <c r="C173" s="6"/>
     </row>
     <row r="174" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B174" s="2"/>
-      <c r="C174" s="2"/>
+      <c r="B174" s="6"/>
+      <c r="C174" s="6"/>
     </row>
     <row r="175" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B175" s="2"/>
-      <c r="C175" s="2"/>
+      <c r="B175" s="6"/>
+      <c r="C175" s="6"/>
     </row>
     <row r="176" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B176" s="2"/>
-      <c r="C176" s="2"/>
+      <c r="B176" s="6"/>
+      <c r="C176" s="6"/>
     </row>
     <row r="177" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B177" s="2"/>
-      <c r="C177" s="2"/>
+      <c r="B177" s="6"/>
+      <c r="C177" s="6"/>
     </row>
     <row r="178" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B178" s="2"/>
-      <c r="C178" s="2"/>
+      <c r="B178" s="6"/>
+      <c r="C178" s="6"/>
     </row>
     <row r="179" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B179" s="2"/>
-      <c r="C179" s="2"/>
+      <c r="B179" s="6"/>
+      <c r="C179" s="6"/>
     </row>
     <row r="180" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B180" s="2"/>
-      <c r="C180" s="2"/>
+      <c r="B180" s="6"/>
+      <c r="C180" s="6"/>
     </row>
     <row r="181" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B181" s="2"/>
-      <c r="C181" s="2"/>
+      <c r="B181" s="6"/>
+      <c r="C181" s="6"/>
     </row>
     <row r="182" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B182" s="2"/>
-      <c r="C182" s="2"/>
+      <c r="B182" s="6"/>
+      <c r="C182" s="6"/>
     </row>
     <row r="183" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B183" s="2"/>
-      <c r="C183" s="2"/>
+      <c r="B183" s="6"/>
+      <c r="C183" s="6"/>
     </row>
     <row r="184" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B184" s="2"/>
-      <c r="C184" s="2"/>
+      <c r="B184" s="6"/>
+      <c r="C184" s="6"/>
     </row>
     <row r="185" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B185" s="2"/>
-      <c r="C185" s="2"/>
+      <c r="B185" s="6"/>
+      <c r="C185" s="6"/>
     </row>
     <row r="186" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B186" s="2"/>
-      <c r="C186" s="2"/>
+      <c r="B186" s="6"/>
+      <c r="C186" s="6"/>
     </row>
     <row r="187" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B187" s="2"/>
-      <c r="C187" s="2"/>
+      <c r="B187" s="6"/>
+      <c r="C187" s="6"/>
     </row>
     <row r="188" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B188" s="2"/>
-      <c r="C188" s="2"/>
+      <c r="B188" s="6"/>
+      <c r="C188" s="6"/>
     </row>
     <row r="189" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B189" s="2"/>
-      <c r="C189" s="2"/>
+      <c r="B189" s="6"/>
+      <c r="C189" s="6"/>
     </row>
     <row r="190" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B190" s="2"/>
-      <c r="C190" s="2"/>
+      <c r="B190" s="6"/>
+      <c r="C190" s="6"/>
     </row>
     <row r="191" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B191" s="2"/>
-      <c r="C191" s="2"/>
+      <c r="B191" s="6"/>
+      <c r="C191" s="6"/>
     </row>
     <row r="192" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B192" s="2"/>
-      <c r="C192" s="2"/>
+      <c r="B192" s="6"/>
+      <c r="C192" s="6"/>
     </row>
     <row r="193" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B193" s="2"/>
-      <c r="C193" s="2"/>
+      <c r="B193" s="6"/>
+      <c r="C193" s="6"/>
     </row>
     <row r="194" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B194" s="2"/>
-      <c r="C194" s="2"/>
+      <c r="B194" s="6"/>
+      <c r="C194" s="6"/>
     </row>
     <row r="195" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B195" s="2"/>
-      <c r="C195" s="2"/>
+      <c r="B195" s="6"/>
+      <c r="C195" s="6"/>
     </row>
     <row r="196" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B196" s="2"/>
-      <c r="C196" s="2"/>
+      <c r="B196" s="6"/>
+      <c r="C196" s="6"/>
     </row>
     <row r="197" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B197" s="2"/>
-      <c r="C197" s="2"/>
+      <c r="B197" s="6"/>
+      <c r="C197" s="6"/>
     </row>
     <row r="198" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B198" s="2"/>
-      <c r="C198" s="2"/>
+      <c r="B198" s="6"/>
+      <c r="C198" s="6"/>
     </row>
     <row r="199" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B199" s="2"/>
-      <c r="C199" s="2"/>
+      <c r="B199" s="6"/>
+      <c r="C199" s="6"/>
     </row>
     <row r="200" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B200" s="2"/>
-      <c r="C200" s="2"/>
+      <c r="B200" s="6"/>
+      <c r="C200" s="6"/>
     </row>
     <row r="201" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B201" s="2"/>
-      <c r="C201" s="2"/>
+      <c r="B201" s="6"/>
+      <c r="C201" s="6"/>
     </row>
     <row r="202" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B202" s="2"/>
-      <c r="C202" s="2"/>
+      <c r="B202" s="6"/>
+      <c r="C202" s="6"/>
     </row>
     <row r="203" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B203" s="2"/>
-      <c r="C203" s="2"/>
+      <c r="B203" s="6"/>
+      <c r="C203" s="6"/>
     </row>
     <row r="204" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B204" s="2"/>
-      <c r="C204" s="2"/>
+      <c r="B204" s="6"/>
+      <c r="C204" s="6"/>
     </row>
     <row r="205" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B205" s="2"/>
-      <c r="C205" s="2"/>
+      <c r="B205" s="6"/>
+      <c r="C205" s="6"/>
     </row>
     <row r="206" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B206" s="2"/>
-      <c r="C206" s="2"/>
+      <c r="B206" s="6"/>
+      <c r="C206" s="6"/>
     </row>
     <row r="207" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B207" s="2"/>
-      <c r="C207" s="2"/>
+      <c r="B207" s="6"/>
+      <c r="C207" s="6"/>
     </row>
     <row r="208" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B208" s="2"/>
-      <c r="C208" s="2"/>
+      <c r="B208" s="6"/>
+      <c r="C208" s="6"/>
     </row>
     <row r="209" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B209" s="2"/>
-      <c r="C209" s="2"/>
+      <c r="B209" s="6"/>
+      <c r="C209" s="6"/>
     </row>
     <row r="210" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B210" s="2"/>
-      <c r="C210" s="2"/>
+      <c r="B210" s="6"/>
+      <c r="C210" s="6"/>
     </row>
     <row r="211" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B211" s="2"/>
-      <c r="C211" s="2"/>
+      <c r="B211" s="6"/>
+      <c r="C211" s="6"/>
     </row>
     <row r="212" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B212" s="2"/>
-      <c r="C212" s="2"/>
+      <c r="B212" s="6"/>
+      <c r="C212" s="6"/>
     </row>
     <row r="213" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B213" s="2"/>
-      <c r="C213" s="2"/>
+      <c r="B213" s="6"/>
+      <c r="C213" s="6"/>
     </row>
     <row r="214" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B214" s="2"/>
-      <c r="C214" s="2"/>
+      <c r="B214" s="6"/>
+      <c r="C214" s="6"/>
     </row>
     <row r="215" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B215" s="2"/>
-      <c r="C215" s="2"/>
+      <c r="B215" s="6"/>
+      <c r="C215" s="6"/>
     </row>
     <row r="216" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B216" s="2"/>
-      <c r="C216" s="2"/>
+      <c r="B216" s="6"/>
+      <c r="C216" s="6"/>
     </row>
     <row r="217" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B217" s="2"/>
-      <c r="C217" s="2"/>
+      <c r="B217" s="6"/>
+      <c r="C217" s="6"/>
     </row>
     <row r="218" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B218" s="2"/>
-      <c r="C218" s="2"/>
+      <c r="B218" s="6"/>
+      <c r="C218" s="6"/>
     </row>
     <row r="219" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B219" s="2"/>
-      <c r="C219" s="2"/>
+      <c r="B219" s="6"/>
+      <c r="C219" s="6"/>
     </row>
     <row r="220" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B220" s="2"/>
-      <c r="C220" s="2"/>
+      <c r="B220" s="6"/>
+      <c r="C220" s="6"/>
     </row>
     <row r="221" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B221" s="2"/>
-      <c r="C221" s="2"/>
+      <c r="B221" s="6"/>
+      <c r="C221" s="6"/>
     </row>
     <row r="222" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B222" s="2"/>
-      <c r="C222" s="2"/>
+      <c r="B222" s="6"/>
+      <c r="C222" s="6"/>
     </row>
     <row r="223" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B223" s="2"/>
-      <c r="C223" s="2"/>
+      <c r="B223" s="6"/>
+      <c r="C223" s="6"/>
     </row>
     <row r="224" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B224" s="2"/>
-      <c r="C224" s="2"/>
+      <c r="B224" s="6"/>
+      <c r="C224" s="6"/>
     </row>
     <row r="225" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B225" s="2"/>
-      <c r="C225" s="2"/>
+      <c r="B225" s="6"/>
+      <c r="C225" s="6"/>
     </row>
     <row r="226" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B226" s="2"/>
-      <c r="C226" s="2"/>
+      <c r="B226" s="6"/>
+      <c r="C226" s="6"/>
     </row>
     <row r="227" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B227" s="2"/>
-      <c r="C227" s="2"/>
+      <c r="B227" s="6"/>
+      <c r="C227" s="6"/>
     </row>
     <row r="228" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B228" s="2"/>
-      <c r="C228" s="2"/>
+      <c r="B228" s="6"/>
+      <c r="C228" s="6"/>
     </row>
     <row r="229" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B229" s="2"/>
-      <c r="C229" s="2"/>
+      <c r="B229" s="6"/>
+      <c r="C229" s="6"/>
     </row>
     <row r="230" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B230" s="2"/>
-      <c r="C230" s="2"/>
+      <c r="B230" s="6"/>
+      <c r="C230" s="6"/>
     </row>
     <row r="231" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B231" s="2"/>
-      <c r="C231" s="2"/>
+      <c r="B231" s="6"/>
+      <c r="C231" s="6"/>
     </row>
     <row r="232" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B232" s="2"/>
-      <c r="C232" s="2"/>
+      <c r="B232" s="6"/>
+      <c r="C232" s="6"/>
     </row>
     <row r="233" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B233" s="2"/>
-      <c r="C233" s="2"/>
+      <c r="B233" s="6"/>
+      <c r="C233" s="6"/>
     </row>
     <row r="234" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B234" s="2"/>
-      <c r="C234" s="2"/>
+      <c r="B234" s="6"/>
+      <c r="C234" s="6"/>
     </row>
     <row r="235" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B235" s="2"/>
-      <c r="C235" s="2"/>
+      <c r="B235" s="6"/>
+      <c r="C235" s="6"/>
     </row>
     <row r="236" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B236" s="2"/>
-      <c r="C236" s="2"/>
+      <c r="B236" s="6"/>
+      <c r="C236" s="6"/>
     </row>
     <row r="237" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B237" s="2"/>
-      <c r="C237" s="2"/>
+      <c r="B237" s="6"/>
+      <c r="C237" s="6"/>
     </row>
     <row r="238" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B238" s="2"/>
-      <c r="C238" s="2"/>
+      <c r="B238" s="6"/>
+      <c r="C238" s="6"/>
     </row>
     <row r="239" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B239" s="2"/>
-      <c r="C239" s="2"/>
+      <c r="B239" s="6"/>
+      <c r="C239" s="6"/>
     </row>
     <row r="240" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B240" s="2"/>
-      <c r="C240" s="2"/>
+      <c r="B240" s="6"/>
+      <c r="C240" s="6"/>
     </row>
     <row r="241" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B241" s="2"/>
-      <c r="C241" s="2"/>
+      <c r="B241" s="6"/>
+      <c r="C241" s="6"/>
     </row>
     <row r="242" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B242" s="2"/>
-      <c r="C242" s="2"/>
+      <c r="B242" s="6"/>
+      <c r="C242" s="6"/>
     </row>
     <row r="243" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B243" s="2"/>
-      <c r="C243" s="2"/>
+      <c r="B243" s="6"/>
+      <c r="C243" s="6"/>
     </row>
     <row r="244" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B244" s="2"/>
-      <c r="C244" s="2"/>
+      <c r="B244" s="6"/>
+      <c r="C244" s="6"/>
     </row>
     <row r="245" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B245" s="2"/>
-      <c r="C245" s="2"/>
+      <c r="B245" s="6"/>
+      <c r="C245" s="6"/>
     </row>
     <row r="246" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B246" s="2"/>
-      <c r="C246" s="2"/>
+      <c r="B246" s="6"/>
+      <c r="C246" s="6"/>
     </row>
     <row r="247" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B247" s="2"/>
-      <c r="C247" s="2"/>
+      <c r="B247" s="6"/>
+      <c r="C247" s="6"/>
     </row>
     <row r="248" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B248" s="2"/>
-      <c r="C248" s="2"/>
+      <c r="B248" s="6"/>
+      <c r="C248" s="6"/>
     </row>
     <row r="249" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B249" s="2"/>
-      <c r="C249" s="2"/>
+      <c r="B249" s="6"/>
+      <c r="C249" s="6"/>
     </row>
     <row r="250" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B250" s="2"/>
-      <c r="C250" s="2"/>
+      <c r="B250" s="6"/>
+      <c r="C250" s="6"/>
     </row>
     <row r="251" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B251" s="2"/>
-      <c r="C251" s="2"/>
+      <c r="B251" s="6"/>
+      <c r="C251" s="6"/>
     </row>
     <row r="252" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B252" s="2"/>
-      <c r="C252" s="2"/>
+      <c r="B252" s="6"/>
+      <c r="C252" s="6"/>
     </row>
     <row r="253" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B253" s="2"/>
-      <c r="C253" s="2"/>
+      <c r="B253" s="6"/>
+      <c r="C253" s="6"/>
     </row>
     <row r="254" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B254" s="2"/>
-      <c r="C254" s="2"/>
+      <c r="B254" s="6"/>
+      <c r="C254" s="6"/>
     </row>
     <row r="255" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B255" s="2"/>
-      <c r="C255" s="2"/>
+      <c r="B255" s="6"/>
+      <c r="C255" s="6"/>
     </row>
     <row r="256" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B256" s="2"/>
-      <c r="C256" s="2"/>
+      <c r="B256" s="6"/>
+      <c r="C256" s="6"/>
     </row>
     <row r="257" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B257" s="2"/>
-      <c r="C257" s="2"/>
+      <c r="B257" s="6"/>
+      <c r="C257" s="6"/>
     </row>
     <row r="258" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B258" s="2"/>
-      <c r="C258" s="2"/>
+      <c r="B258" s="6"/>
+      <c r="C258" s="6"/>
     </row>
     <row r="259" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B259" s="2"/>
-      <c r="C259" s="2"/>
+      <c r="B259" s="6"/>
+      <c r="C259" s="6"/>
     </row>
     <row r="260" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B260" s="2"/>
-      <c r="C260" s="2"/>
+      <c r="B260" s="6"/>
+      <c r="C260" s="6"/>
     </row>
     <row r="261" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B261" s="2"/>
-      <c r="C261" s="2"/>
+      <c r="B261" s="6"/>
+      <c r="C261" s="6"/>
     </row>
     <row r="262" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B262" s="2"/>
-      <c r="C262" s="2"/>
+      <c r="B262" s="6"/>
+      <c r="C262" s="6"/>
     </row>
     <row r="263" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B263" s="2"/>
-      <c r="C263" s="2"/>
+      <c r="B263" s="6"/>
+      <c r="C263" s="6"/>
     </row>
     <row r="264" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B264" s="2"/>
-      <c r="C264" s="2"/>
+      <c r="B264" s="6"/>
+      <c r="C264" s="6"/>
     </row>
     <row r="265" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B265" s="2"/>
-      <c r="C265" s="2"/>
+      <c r="B265" s="6"/>
+      <c r="C265" s="6"/>
     </row>
     <row r="266" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B266" s="2"/>
-      <c r="C266" s="2"/>
+      <c r="B266" s="6"/>
+      <c r="C266" s="6"/>
     </row>
     <row r="267" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B267" s="2"/>
-      <c r="C267" s="2"/>
+      <c r="B267" s="6"/>
+      <c r="C267" s="6"/>
     </row>
     <row r="268" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B268" s="2"/>
-      <c r="C268" s="2"/>
+      <c r="B268" s="6"/>
+      <c r="C268" s="6"/>
     </row>
     <row r="269" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B269" s="2"/>
-      <c r="C269" s="2"/>
+      <c r="B269" s="6"/>
+      <c r="C269" s="6"/>
     </row>
     <row r="270" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B270" s="2"/>
-      <c r="C270" s="2"/>
+      <c r="B270" s="6"/>
+      <c r="C270" s="6"/>
     </row>
     <row r="271" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B271" s="2"/>
-      <c r="C271" s="2"/>
+      <c r="B271" s="6"/>
+      <c r="C271" s="6"/>
     </row>
     <row r="272" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B272" s="2"/>
-      <c r="C272" s="2"/>
+      <c r="B272" s="6"/>
+      <c r="C272" s="6"/>
     </row>
     <row r="273" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B273" s="2"/>
-      <c r="C273" s="2"/>
+      <c r="B273" s="6"/>
+      <c r="C273" s="6"/>
     </row>
     <row r="274" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B274" s="2"/>
-      <c r="C274" s="2"/>
+      <c r="B274" s="6"/>
+      <c r="C274" s="6"/>
     </row>
     <row r="275" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B275" s="2"/>
-      <c r="C275" s="2"/>
+      <c r="B275" s="6"/>
+      <c r="C275" s="6"/>
     </row>
     <row r="276" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B276" s="2"/>
-      <c r="C276" s="2"/>
+      <c r="B276" s="6"/>
+      <c r="C276" s="6"/>
     </row>
     <row r="277" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B277" s="2"/>
-      <c r="C277" s="2"/>
+      <c r="B277" s="6"/>
+      <c r="C277" s="6"/>
     </row>
     <row r="278" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B278" s="2"/>
-      <c r="C278" s="2"/>
+      <c r="B278" s="6"/>
+      <c r="C278" s="6"/>
     </row>
     <row r="279" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B279" s="2"/>
-      <c r="C279" s="2"/>
+      <c r="B279" s="6"/>
+      <c r="C279" s="6"/>
     </row>
     <row r="280" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B280" s="2"/>
-      <c r="C280" s="2"/>
+      <c r="B280" s="6"/>
+      <c r="C280" s="6"/>
     </row>
     <row r="281" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B281" s="2"/>
-      <c r="C281" s="2"/>
+      <c r="B281" s="6"/>
+      <c r="C281" s="6"/>
     </row>
     <row r="282" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B282" s="2"/>
-      <c r="C282" s="2"/>
+      <c r="B282" s="6"/>
+      <c r="C282" s="6"/>
     </row>
     <row r="283" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B283" s="2"/>
-      <c r="C283" s="2"/>
+      <c r="B283" s="6"/>
+      <c r="C283" s="6"/>
     </row>
     <row r="284" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B284" s="2"/>
-      <c r="C284" s="2"/>
+      <c r="B284" s="6"/>
+      <c r="C284" s="6"/>
     </row>
     <row r="285" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B285" s="2"/>
-      <c r="C285" s="2"/>
+      <c r="B285" s="6"/>
+      <c r="C285" s="6"/>
     </row>
     <row r="286" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B286" s="2"/>
-      <c r="C286" s="2"/>
+      <c r="B286" s="6"/>
+      <c r="C286" s="6"/>
     </row>
     <row r="287" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B287" s="2"/>
-      <c r="C287" s="2"/>
+      <c r="B287" s="6"/>
+      <c r="C287" s="6"/>
     </row>
     <row r="288" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B288" s="2"/>
-      <c r="C288" s="2"/>
+      <c r="B288" s="6"/>
+      <c r="C288" s="6"/>
     </row>
     <row r="289" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B289" s="2"/>
-      <c r="C289" s="2"/>
+      <c r="B289" s="6"/>
+      <c r="C289" s="6"/>
     </row>
     <row r="290" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B290" s="2"/>
-      <c r="C290" s="2"/>
+      <c r="B290" s="6"/>
+      <c r="C290" s="6"/>
     </row>
     <row r="291" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B291" s="2"/>
-      <c r="C291" s="2"/>
+      <c r="B291" s="6"/>
+      <c r="C291" s="6"/>
     </row>
     <row r="292" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B292" s="2"/>
-      <c r="C292" s="2"/>
+      <c r="B292" s="6"/>
+      <c r="C292" s="6"/>
     </row>
     <row r="293" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B293" s="2"/>
-      <c r="C293" s="2"/>
+      <c r="B293" s="6"/>
+      <c r="C293" s="6"/>
     </row>
     <row r="294" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B294" s="2"/>
-      <c r="C294" s="2"/>
+      <c r="B294" s="6"/>
+      <c r="C294" s="6"/>
     </row>
     <row r="295" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B295" s="2"/>
-      <c r="C295" s="2"/>
+      <c r="B295" s="6"/>
+      <c r="C295" s="6"/>
     </row>
     <row r="296" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B296" s="2"/>
-      <c r="C296" s="2"/>
+      <c r="B296" s="6"/>
+      <c r="C296" s="6"/>
     </row>
     <row r="297" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B297" s="2"/>
-      <c r="C297" s="2"/>
+      <c r="B297" s="6"/>
+      <c r="C297" s="6"/>
     </row>
     <row r="298" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B298" s="2"/>
-      <c r="C298" s="2"/>
+      <c r="B298" s="6"/>
+      <c r="C298" s="6"/>
     </row>
     <row r="299" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B299" s="2"/>
-      <c r="C299" s="2"/>
+      <c r="B299" s="6"/>
+      <c r="C299" s="6"/>
     </row>
     <row r="300" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B300" s="2"/>
-      <c r="C300" s="2"/>
+      <c r="B300" s="6"/>
+      <c r="C300" s="6"/>
     </row>
     <row r="301" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B301" s="2"/>
-      <c r="C301" s="2"/>
+      <c r="B301" s="6"/>
+      <c r="C301" s="6"/>
     </row>
     <row r="302" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B302" s="2"/>
-      <c r="C302" s="2"/>
+      <c r="B302" s="6"/>
+      <c r="C302" s="6"/>
     </row>
     <row r="303" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B303" s="2"/>
-      <c r="C303" s="2"/>
+      <c r="B303" s="6"/>
+      <c r="C303" s="6"/>
     </row>
     <row r="304" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B304" s="2"/>
-      <c r="C304" s="2"/>
+      <c r="B304" s="6"/>
+      <c r="C304" s="6"/>
     </row>
     <row r="305" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B305" s="2"/>
-      <c r="C305" s="2"/>
+      <c r="B305" s="6"/>
+      <c r="C305" s="6"/>
     </row>
     <row r="306" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B306" s="2"/>
-      <c r="C306" s="2"/>
+      <c r="B306" s="6"/>
+      <c r="C306" s="6"/>
     </row>
     <row r="307" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B307" s="2"/>
-      <c r="C307" s="2"/>
+      <c r="B307" s="6"/>
+      <c r="C307" s="6"/>
     </row>
     <row r="308" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B308" s="2"/>
-      <c r="C308" s="2"/>
+      <c r="B308" s="6"/>
+      <c r="C308" s="6"/>
     </row>
     <row r="309" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B309" s="2"/>
-      <c r="C309" s="2"/>
+      <c r="B309" s="6"/>
+      <c r="C309" s="6"/>
     </row>
     <row r="310" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B310" s="2"/>
-      <c r="C310" s="2"/>
+      <c r="B310" s="6"/>
+      <c r="C310" s="6"/>
     </row>
     <row r="311" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B311" s="2"/>
-      <c r="C311" s="2"/>
+      <c r="B311" s="6"/>
+      <c r="C311" s="6"/>
     </row>
     <row r="312" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B312" s="2"/>
-      <c r="C312" s="2"/>
+      <c r="B312" s="6"/>
+      <c r="C312" s="6"/>
     </row>
     <row r="313" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B313" s="2"/>
-      <c r="C313" s="2"/>
+      <c r="B313" s="6"/>
+      <c r="C313" s="6"/>
     </row>
     <row r="314" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B314" s="2"/>
-      <c r="C314" s="2"/>
+      <c r="B314" s="6"/>
+      <c r="C314" s="6"/>
     </row>
     <row r="315" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B315" s="2"/>
-      <c r="C315" s="2"/>
+      <c r="B315" s="6"/>
+      <c r="C315" s="6"/>
     </row>
     <row r="316" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B316" s="2"/>
-      <c r="C316" s="2"/>
+      <c r="B316" s="6"/>
+      <c r="C316" s="6"/>
     </row>
     <row r="317" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B317" s="2"/>
-      <c r="C317" s="2"/>
+      <c r="B317" s="6"/>
+      <c r="C317" s="6"/>
     </row>
     <row r="318" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B318" s="2"/>
-      <c r="C318" s="2"/>
+      <c r="B318" s="6"/>
+      <c r="C318" s="6"/>
     </row>
     <row r="319" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B319" s="2"/>
-      <c r="C319" s="2"/>
+      <c r="B319" s="6"/>
+      <c r="C319" s="6"/>
     </row>
     <row r="320" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B320" s="2"/>
-      <c r="C320" s="2"/>
+      <c r="B320" s="6"/>
+      <c r="C320" s="6"/>
     </row>
     <row r="321" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B321" s="2"/>
-      <c r="C321" s="2"/>
+      <c r="B321" s="6"/>
+      <c r="C321" s="6"/>
     </row>
     <row r="322" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B322" s="2"/>
-      <c r="C322" s="2"/>
+      <c r="B322" s="6"/>
+      <c r="C322" s="6"/>
     </row>
     <row r="323" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B323" s="2"/>
-      <c r="C323" s="2"/>
+      <c r="B323" s="6"/>
+      <c r="C323" s="6"/>
     </row>
     <row r="324" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B324" s="2"/>
-      <c r="C324" s="2"/>
+      <c r="B324" s="6"/>
+      <c r="C324" s="6"/>
     </row>
     <row r="325" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B325" s="2"/>
-      <c r="C325" s="2"/>
+      <c r="B325" s="6"/>
+      <c r="C325" s="6"/>
     </row>
     <row r="326" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B326" s="2"/>
-      <c r="C326" s="2"/>
+      <c r="B326" s="6"/>
+      <c r="C326" s="6"/>
     </row>
     <row r="327" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B327" s="2"/>
-      <c r="C327" s="2"/>
+      <c r="B327" s="6"/>
+      <c r="C327" s="6"/>
     </row>
     <row r="328" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B328" s="2"/>
-      <c r="C328" s="2"/>
+      <c r="B328" s="6"/>
+      <c r="C328" s="6"/>
     </row>
     <row r="329" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B329" s="2"/>
-      <c r="C329" s="2"/>
+      <c r="B329" s="6"/>
+      <c r="C329" s="6"/>
     </row>
     <row r="330" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B330" s="2"/>
-      <c r="C330" s="2"/>
+      <c r="B330" s="6"/>
+      <c r="C330" s="6"/>
     </row>
     <row r="331" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B331" s="2"/>
-      <c r="C331" s="2"/>
+      <c r="B331" s="6"/>
+      <c r="C331" s="6"/>
     </row>
     <row r="332" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B332" s="2"/>
-      <c r="C332" s="2"/>
+      <c r="B332" s="6"/>
+      <c r="C332" s="6"/>
     </row>
     <row r="333" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B333" s="2"/>
-      <c r="C333" s="2"/>
+      <c r="B333" s="6"/>
+      <c r="C333" s="6"/>
     </row>
     <row r="334" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B334" s="2"/>
-      <c r="C334" s="2"/>
+      <c r="B334" s="6"/>
+      <c r="C334" s="6"/>
     </row>
     <row r="335" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B335" s="2"/>
-      <c r="C335" s="2"/>
+      <c r="B335" s="6"/>
+      <c r="C335" s="6"/>
     </row>
     <row r="336" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B336" s="2"/>
-      <c r="C336" s="2"/>
+      <c r="B336" s="6"/>
+      <c r="C336" s="6"/>
     </row>
     <row r="337" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B337" s="2"/>
-      <c r="C337" s="2"/>
+      <c r="B337" s="6"/>
+      <c r="C337" s="6"/>
     </row>
     <row r="338" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B338" s="2"/>
-      <c r="C338" s="2"/>
+      <c r="B338" s="6"/>
+      <c r="C338" s="6"/>
     </row>
     <row r="339" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B339" s="2"/>
-      <c r="C339" s="2"/>
+      <c r="B339" s="6"/>
+      <c r="C339" s="6"/>
     </row>
     <row r="340" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B340" s="2"/>
-      <c r="C340" s="2"/>
+      <c r="B340" s="6"/>
+      <c r="C340" s="6"/>
     </row>
     <row r="341" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B341" s="2"/>
-      <c r="C341" s="2"/>
+      <c r="B341" s="6"/>
+      <c r="C341" s="6"/>
     </row>
     <row r="342" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B342" s="2"/>
-      <c r="C342" s="2"/>
+      <c r="B342" s="6"/>
+      <c r="C342" s="6"/>
     </row>
     <row r="343" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B343" s="2"/>
-      <c r="C343" s="2"/>
+      <c r="B343" s="6"/>
+      <c r="C343" s="6"/>
     </row>
     <row r="344" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B344" s="2"/>
-      <c r="C344" s="2"/>
+      <c r="B344" s="6"/>
+      <c r="C344" s="6"/>
     </row>
     <row r="345" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B345" s="2"/>
-      <c r="C345" s="2"/>
+      <c r="B345" s="6"/>
+      <c r="C345" s="6"/>
     </row>
     <row r="346" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B346" s="2"/>
-      <c r="C346" s="2"/>
+      <c r="B346" s="6"/>
+      <c r="C346" s="6"/>
     </row>
     <row r="347" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B347" s="2"/>
-      <c r="C347" s="2"/>
+      <c r="B347" s="6"/>
+      <c r="C347" s="6"/>
     </row>
     <row r="348" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B348" s="2"/>
-      <c r="C348" s="2"/>
+      <c r="B348" s="6"/>
+      <c r="C348" s="6"/>
     </row>
     <row r="349" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B349" s="2"/>
-      <c r="C349" s="2"/>
+      <c r="B349" s="6"/>
+      <c r="C349" s="6"/>
     </row>
     <row r="350" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B350" s="2"/>
-      <c r="C350" s="2"/>
+      <c r="B350" s="6"/>
+      <c r="C350" s="6"/>
     </row>
     <row r="351" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B351" s="2"/>
-      <c r="C351" s="2"/>
+      <c r="B351" s="6"/>
+      <c r="C351" s="6"/>
     </row>
     <row r="352" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B352" s="2"/>
-      <c r="C352" s="2"/>
+      <c r="B352" s="6"/>
+      <c r="C352" s="6"/>
     </row>
     <row r="353" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B353" s="2"/>
-      <c r="C353" s="2"/>
+      <c r="B353" s="6"/>
+      <c r="C353" s="6"/>
     </row>
     <row r="354" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B354" s="2"/>
-      <c r="C354" s="2"/>
+      <c r="B354" s="6"/>
+      <c r="C354" s="6"/>
     </row>
     <row r="355" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B355" s="2"/>
-      <c r="C355" s="2"/>
+      <c r="B355" s="6"/>
+      <c r="C355" s="6"/>
     </row>
     <row r="356" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B356" s="2"/>
-      <c r="C356" s="2"/>
+      <c r="B356" s="6"/>
+      <c r="C356" s="6"/>
     </row>
     <row r="357" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B357" s="2"/>
-      <c r="C357" s="2"/>
+      <c r="B357" s="6"/>
+      <c r="C357" s="6"/>
     </row>
     <row r="358" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B358" s="2"/>
-      <c r="C358" s="2"/>
+      <c r="B358" s="6"/>
+      <c r="C358" s="6"/>
     </row>
     <row r="359" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B359" s="2"/>
-      <c r="C359" s="2"/>
+      <c r="B359" s="6"/>
+      <c r="C359" s="6"/>
     </row>
     <row r="360" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B360" s="2"/>
-      <c r="C360" s="2"/>
+      <c r="B360" s="6"/>
+      <c r="C360" s="6"/>
     </row>
     <row r="361" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B361" s="2"/>
-      <c r="C361" s="2"/>
+      <c r="B361" s="6"/>
+      <c r="C361" s="6"/>
     </row>
     <row r="362" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B362" s="2"/>
-      <c r="C362" s="2"/>
+      <c r="B362" s="6"/>
+      <c r="C362" s="6"/>
     </row>
     <row r="363" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B363" s="2"/>
-      <c r="C363" s="2"/>
+      <c r="B363" s="6"/>
+      <c r="C363" s="6"/>
     </row>
     <row r="364" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B364" s="2"/>
-      <c r="C364" s="2"/>
+      <c r="B364" s="6"/>
+      <c r="C364" s="6"/>
     </row>
     <row r="365" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B365" s="2"/>
-      <c r="C365" s="2"/>
+      <c r="B365" s="6"/>
+      <c r="C365" s="6"/>
     </row>
     <row r="366" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B366" s="2"/>
-      <c r="C366" s="2"/>
+      <c r="B366" s="6"/>
+      <c r="C366" s="6"/>
     </row>
     <row r="367" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B367" s="2"/>
-      <c r="C367" s="2"/>
+      <c r="B367" s="6"/>
+      <c r="C367" s="6"/>
     </row>
     <row r="368" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B368" s="2"/>
-      <c r="C368" s="2"/>
+      <c r="B368" s="6"/>
+      <c r="C368" s="6"/>
     </row>
     <row r="369" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B369" s="2"/>
-      <c r="C369" s="2"/>
+      <c r="B369" s="6"/>
+      <c r="C369" s="6"/>
     </row>
     <row r="370" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B370" s="2"/>
-      <c r="C370" s="2"/>
+      <c r="B370" s="6"/>
+      <c r="C370" s="6"/>
     </row>
     <row r="371" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B371" s="2"/>
-      <c r="C371" s="2"/>
+      <c r="B371" s="6"/>
+      <c r="C371" s="6"/>
     </row>
     <row r="372" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B372" s="2"/>
-      <c r="C372" s="2"/>
+      <c r="B372" s="6"/>
+      <c r="C372" s="6"/>
     </row>
     <row r="373" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B373" s="2"/>
-      <c r="C373" s="2"/>
+      <c r="B373" s="6"/>
+      <c r="C373" s="6"/>
     </row>
     <row r="374" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B374" s="2"/>
-      <c r="C374" s="2"/>
+      <c r="B374" s="6"/>
+      <c r="C374" s="6"/>
     </row>
     <row r="375" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B375" s="2"/>
-      <c r="C375" s="2"/>
+      <c r="B375" s="6"/>
+      <c r="C375" s="6"/>
     </row>
     <row r="376" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B376" s="2"/>
-      <c r="C376" s="2"/>
+      <c r="B376" s="6"/>
+      <c r="C376" s="6"/>
     </row>
     <row r="377" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B377" s="2"/>
-      <c r="C377" s="2"/>
+      <c r="B377" s="6"/>
+      <c r="C377" s="6"/>
     </row>
     <row r="378" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B378" s="2"/>
-      <c r="C378" s="2"/>
+      <c r="B378" s="6"/>
+      <c r="C378" s="6"/>
     </row>
     <row r="379" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B379" s="2"/>
-      <c r="C379" s="2"/>
+      <c r="B379" s="6"/>
+      <c r="C379" s="6"/>
     </row>
     <row r="380" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B380" s="2"/>
-      <c r="C380" s="2"/>
+      <c r="B380" s="6"/>
+      <c r="C380" s="6"/>
     </row>
     <row r="381" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B381" s="2"/>
-      <c r="C381" s="2"/>
+      <c r="B381" s="6"/>
+      <c r="C381" s="6"/>
     </row>
     <row r="382" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B382" s="2"/>
-      <c r="C382" s="2"/>
+      <c r="B382" s="6"/>
+      <c r="C382" s="6"/>
     </row>
     <row r="383" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B383" s="2"/>
-      <c r="C383" s="2"/>
+      <c r="B383" s="6"/>
+      <c r="C383" s="6"/>
     </row>
     <row r="384" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B384" s="2"/>
-      <c r="C384" s="2"/>
+      <c r="B384" s="6"/>
+      <c r="C384" s="6"/>
     </row>
     <row r="385" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B385" s="2"/>
-      <c r="C385" s="2"/>
+      <c r="B385" s="6"/>
+      <c r="C385" s="6"/>
     </row>
     <row r="386" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B386" s="2"/>
-      <c r="C386" s="2"/>
+      <c r="B386" s="6"/>
+      <c r="C386" s="6"/>
     </row>
     <row r="387" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B387" s="2"/>
-      <c r="C387" s="2"/>
+      <c r="B387" s="6"/>
+      <c r="C387" s="6"/>
     </row>
     <row r="388" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B388" s="2"/>
-      <c r="C388" s="2"/>
+      <c r="B388" s="6"/>
+      <c r="C388" s="6"/>
     </row>
     <row r="389" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B389" s="2"/>
-      <c r="C389" s="2"/>
+      <c r="B389" s="6"/>
+      <c r="C389" s="6"/>
     </row>
     <row r="390" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B390" s="2"/>
-      <c r="C390" s="2"/>
+      <c r="B390" s="6"/>
+      <c r="C390" s="6"/>
     </row>
     <row r="391" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B391" s="2"/>
-      <c r="C391" s="2"/>
+      <c r="B391" s="6"/>
+      <c r="C391" s="6"/>
     </row>
     <row r="392" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B392" s="2"/>
-      <c r="C392" s="2"/>
+      <c r="B392" s="6"/>
+      <c r="C392" s="6"/>
     </row>
     <row r="393" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B393" s="2"/>
-      <c r="C393" s="2"/>
+      <c r="B393" s="6"/>
+      <c r="C393" s="6"/>
     </row>
     <row r="394" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B394" s="2"/>
-      <c r="C394" s="2"/>
+      <c r="B394" s="6"/>
+      <c r="C394" s="6"/>
     </row>
     <row r="395" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B395" s="2"/>
-      <c r="C395" s="2"/>
+      <c r="B395" s="6"/>
+      <c r="C395" s="6"/>
     </row>
     <row r="396" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B396" s="2"/>
-      <c r="C396" s="2"/>
+      <c r="B396" s="6"/>
+      <c r="C396" s="6"/>
     </row>
     <row r="397" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B397" s="2"/>
-      <c r="C397" s="2"/>
+      <c r="B397" s="6"/>
+      <c r="C397" s="6"/>
     </row>
     <row r="398" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B398" s="2"/>
-      <c r="C398" s="2"/>
+      <c r="B398" s="6"/>
+      <c r="C398" s="6"/>
     </row>
     <row r="399" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B399" s="2"/>
-      <c r="C399" s="2"/>
+      <c r="B399" s="6"/>
+      <c r="C399" s="6"/>
     </row>
     <row r="400" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B400" s="2"/>
-      <c r="C400" s="2"/>
+      <c r="B400" s="6"/>
+      <c r="C400" s="6"/>
     </row>
     <row r="401" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B401" s="2"/>
-      <c r="C401" s="2"/>
+      <c r="B401" s="6"/>
+      <c r="C401" s="6"/>
     </row>
     <row r="402" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B402" s="2"/>
-      <c r="C402" s="2"/>
+      <c r="B402" s="6"/>
+      <c r="C402" s="6"/>
     </row>
     <row r="403" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B403" s="2"/>
-      <c r="C403" s="2"/>
+      <c r="B403" s="6"/>
+      <c r="C403" s="6"/>
     </row>
     <row r="404" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B404" s="2"/>
-      <c r="C404" s="2"/>
+      <c r="B404" s="6"/>
+      <c r="C404" s="6"/>
     </row>
     <row r="405" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B405" s="2"/>
-      <c r="C405" s="2"/>
+      <c r="B405" s="6"/>
+      <c r="C405" s="6"/>
     </row>
     <row r="406" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B406" s="2"/>
-      <c r="C406" s="2"/>
+      <c r="B406" s="6"/>
+      <c r="C406" s="6"/>
     </row>
     <row r="407" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B407" s="2"/>
-      <c r="C407" s="2"/>
+      <c r="B407" s="6"/>
+      <c r="C407" s="6"/>
     </row>
     <row r="408" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B408" s="2"/>
-      <c r="C408" s="2"/>
+      <c r="B408" s="6"/>
+      <c r="C408" s="6"/>
     </row>
     <row r="409" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B409" s="2"/>
-      <c r="C409" s="2"/>
+      <c r="B409" s="6"/>
+      <c r="C409" s="6"/>
     </row>
     <row r="410" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B410" s="2"/>
-      <c r="C410" s="2"/>
+      <c r="B410" s="6"/>
+      <c r="C410" s="6"/>
     </row>
     <row r="411" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B411" s="2"/>
-      <c r="C411" s="2"/>
+      <c r="B411" s="6"/>
+      <c r="C411" s="6"/>
     </row>
     <row r="412" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B412" s="2"/>
-      <c r="C412" s="2"/>
+      <c r="B412" s="6"/>
+      <c r="C412" s="6"/>
     </row>
     <row r="413" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B413" s="2"/>
-      <c r="C413" s="2"/>
+      <c r="B413" s="6"/>
+      <c r="C413" s="6"/>
     </row>
     <row r="414" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B414" s="2"/>
-      <c r="C414" s="2"/>
+      <c r="B414" s="6"/>
+      <c r="C414" s="6"/>
     </row>
     <row r="415" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B415" s="2"/>
-      <c r="C415" s="2"/>
+      <c r="B415" s="6"/>
+      <c r="C415" s="6"/>
     </row>
     <row r="416" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B416" s="2"/>
-      <c r="C416" s="2"/>
+      <c r="B416" s="6"/>
+      <c r="C416" s="6"/>
     </row>
     <row r="417" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B417" s="2"/>
-      <c r="C417" s="2"/>
+      <c r="B417" s="6"/>
+      <c r="C417" s="6"/>
     </row>
     <row r="418" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B418" s="2"/>
-      <c r="C418" s="2"/>
+      <c r="B418" s="6"/>
+      <c r="C418" s="6"/>
     </row>
     <row r="419" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B419" s="2"/>
-      <c r="C419" s="2"/>
+      <c r="B419" s="6"/>
+      <c r="C419" s="6"/>
     </row>
     <row r="420" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B420" s="2"/>
-      <c r="C420" s="2"/>
+      <c r="B420" s="6"/>
+      <c r="C420" s="6"/>
     </row>
     <row r="421" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B421" s="2"/>
-      <c r="C421" s="2"/>
+      <c r="B421" s="6"/>
+      <c r="C421" s="6"/>
     </row>
     <row r="422" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B422" s="2"/>
-      <c r="C422" s="2"/>
+      <c r="B422" s="6"/>
+      <c r="C422" s="6"/>
     </row>
     <row r="423" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B423" s="2"/>
-      <c r="C423" s="2"/>
+      <c r="B423" s="6"/>
+      <c r="C423" s="6"/>
     </row>
     <row r="424" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B424" s="2"/>
-      <c r="C424" s="2"/>
+      <c r="B424" s="6"/>
+      <c r="C424" s="6"/>
     </row>
     <row r="425" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B425" s="2"/>
-      <c r="C425" s="2"/>
+      <c r="B425" s="6"/>
+      <c r="C425" s="6"/>
     </row>
     <row r="426" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B426" s="2"/>
-      <c r="C426" s="2"/>
+      <c r="B426" s="6"/>
+      <c r="C426" s="6"/>
     </row>
     <row r="427" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B427" s="2"/>
-      <c r="C427" s="2"/>
+      <c r="B427" s="6"/>
+      <c r="C427" s="6"/>
     </row>
     <row r="428" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B428" s="2"/>
-      <c r="C428" s="2"/>
+      <c r="B428" s="6"/>
+      <c r="C428" s="6"/>
     </row>
     <row r="429" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B429" s="2"/>
-      <c r="C429" s="2"/>
+      <c r="B429" s="6"/>
+      <c r="C429" s="6"/>
     </row>
     <row r="430" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B430" s="2"/>
-      <c r="C430" s="2"/>
+      <c r="B430" s="6"/>
+      <c r="C430" s="6"/>
     </row>
     <row r="431" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B431" s="2"/>
-      <c r="C431" s="2"/>
+      <c r="B431" s="6"/>
+      <c r="C431" s="6"/>
     </row>
     <row r="432" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B432" s="2"/>
-      <c r="C432" s="2"/>
+      <c r="B432" s="6"/>
+      <c r="C432" s="6"/>
     </row>
     <row r="433" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B433" s="2"/>
-      <c r="C433" s="2"/>
+      <c r="B433" s="6"/>
+      <c r="C433" s="6"/>
     </row>
     <row r="434" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B434" s="2"/>
-      <c r="C434" s="2"/>
+      <c r="B434" s="6"/>
+      <c r="C434" s="6"/>
     </row>
     <row r="435" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B435" s="2"/>
-      <c r="C435" s="2"/>
+      <c r="B435" s="6"/>
+      <c r="C435" s="6"/>
     </row>
     <row r="436" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B436" s="2"/>
-      <c r="C436" s="2"/>
+      <c r="B436" s="6"/>
+      <c r="C436" s="6"/>
     </row>
     <row r="437" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B437" s="2"/>
-      <c r="C437" s="2"/>
+      <c r="B437" s="6"/>
+      <c r="C437" s="6"/>
     </row>
     <row r="438" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B438" s="2"/>
-      <c r="C438" s="2"/>
+      <c r="B438" s="6"/>
+      <c r="C438" s="6"/>
     </row>
     <row r="439" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B439" s="2"/>
-      <c r="C439" s="2"/>
+      <c r="B439" s="6"/>
+      <c r="C439" s="6"/>
     </row>
     <row r="440" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B440" s="2"/>
-      <c r="C440" s="2"/>
+      <c r="B440" s="6"/>
+      <c r="C440" s="6"/>
     </row>
     <row r="441" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B441" s="2"/>
-      <c r="C441" s="2"/>
+      <c r="B441" s="6"/>
+      <c r="C441" s="6"/>
     </row>
     <row r="442" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B442" s="2"/>
-      <c r="C442" s="2"/>
+      <c r="B442" s="6"/>
+      <c r="C442" s="6"/>
     </row>
     <row r="443" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B443" s="2"/>
-      <c r="C443" s="2"/>
+      <c r="B443" s="6"/>
+      <c r="C443" s="6"/>
     </row>
     <row r="444" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B444" s="2"/>
-      <c r="C444" s="2"/>
+      <c r="B444" s="6"/>
+      <c r="C444" s="6"/>
     </row>
     <row r="445" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B445" s="2"/>
-      <c r="C445" s="2"/>
+      <c r="B445" s="6"/>
+      <c r="C445" s="6"/>
     </row>
     <row r="446" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B446" s="2"/>
-      <c r="C446" s="2"/>
+      <c r="B446" s="6"/>
+      <c r="C446" s="6"/>
     </row>
     <row r="447" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B447" s="2"/>
-      <c r="C447" s="2"/>
+      <c r="B447" s="6"/>
+      <c r="C447" s="6"/>
     </row>
     <row r="448" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B448" s="2"/>
-      <c r="C448" s="2"/>
+      <c r="B448" s="6"/>
+      <c r="C448" s="6"/>
     </row>
     <row r="449" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B449" s="2"/>
-      <c r="C449" s="2"/>
+      <c r="B449" s="6"/>
+      <c r="C449" s="6"/>
     </row>
     <row r="450" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B450" s="2"/>
-      <c r="C450" s="2"/>
+      <c r="B450" s="6"/>
+      <c r="C450" s="6"/>
     </row>
     <row r="451" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B451" s="2"/>
-      <c r="C451" s="2"/>
+      <c r="B451" s="6"/>
+      <c r="C451" s="6"/>
     </row>
     <row r="452" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B452" s="2"/>
-      <c r="C452" s="2"/>
+      <c r="B452" s="6"/>
+      <c r="C452" s="6"/>
     </row>
     <row r="453" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B453" s="2"/>
-      <c r="C453" s="2"/>
+      <c r="B453" s="6"/>
+      <c r="C453" s="6"/>
     </row>
     <row r="454" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B454" s="2"/>
-      <c r="C454" s="2"/>
+      <c r="B454" s="6"/>
+      <c r="C454" s="6"/>
     </row>
     <row r="455" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B455" s="2"/>
-      <c r="C455" s="2"/>
+      <c r="B455" s="6"/>
+      <c r="C455" s="6"/>
     </row>
     <row r="456" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B456" s="2"/>
-      <c r="C456" s="2"/>
+      <c r="B456" s="6"/>
+      <c r="C456" s="6"/>
     </row>
     <row r="457" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B457" s="2"/>
-      <c r="C457" s="2"/>
+      <c r="B457" s="6"/>
+      <c r="C457" s="6"/>
     </row>
     <row r="458" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B458" s="2"/>
-      <c r="C458" s="2"/>
+      <c r="B458" s="6"/>
+      <c r="C458" s="6"/>
     </row>
     <row r="459" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B459" s="2"/>
-      <c r="C459" s="2"/>
+      <c r="B459" s="6"/>
+      <c r="C459" s="6"/>
     </row>
     <row r="460" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B460" s="2"/>
-      <c r="C460" s="2"/>
+      <c r="B460" s="6"/>
+      <c r="C460" s="6"/>
     </row>
     <row r="461" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B461" s="2"/>
-      <c r="C461" s="2"/>
+      <c r="B461" s="6"/>
+      <c r="C461" s="6"/>
     </row>
     <row r="462" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B462" s="2"/>
-      <c r="C462" s="2"/>
+      <c r="B462" s="6"/>
+      <c r="C462" s="6"/>
     </row>
     <row r="463" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B463" s="2"/>
-      <c r="C463" s="2"/>
+      <c r="B463" s="6"/>
+      <c r="C463" s="6"/>
     </row>
     <row r="464" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B464" s="2"/>
-      <c r="C464" s="2"/>
+      <c r="B464" s="6"/>
+      <c r="C464" s="6"/>
     </row>
     <row r="465" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B465" s="2"/>
-      <c r="C465" s="2"/>
+      <c r="B465" s="6"/>
+      <c r="C465" s="6"/>
     </row>
     <row r="466" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B466" s="2"/>
-      <c r="C466" s="2"/>
+      <c r="B466" s="6"/>
+      <c r="C466" s="6"/>
     </row>
     <row r="467" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B467" s="2"/>
-      <c r="C467" s="2"/>
+      <c r="B467" s="6"/>
+      <c r="C467" s="6"/>
     </row>
     <row r="468" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B468" s="2"/>
-      <c r="C468" s="2"/>
+      <c r="B468" s="6"/>
+      <c r="C468" s="6"/>
     </row>
     <row r="469" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B469" s="2"/>
-      <c r="C469" s="2"/>
+      <c r="B469" s="6"/>
+      <c r="C469" s="6"/>
     </row>
     <row r="470" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B470" s="2"/>
-      <c r="C470" s="2"/>
+      <c r="B470" s="6"/>
+      <c r="C470" s="6"/>
     </row>
     <row r="471" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B471" s="2"/>
-      <c r="C471" s="2"/>
+      <c r="B471" s="6"/>
+      <c r="C471" s="6"/>
     </row>
     <row r="472" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B472" s="2"/>
-      <c r="C472" s="2"/>
+      <c r="B472" s="6"/>
+      <c r="C472" s="6"/>
     </row>
     <row r="473" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B473" s="2"/>
-      <c r="C473" s="2"/>
+      <c r="B473" s="6"/>
+      <c r="C473" s="6"/>
     </row>
     <row r="474" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B474" s="2"/>
-      <c r="C474" s="2"/>
+      <c r="B474" s="6"/>
+      <c r="C474" s="6"/>
     </row>
     <row r="475" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B475" s="2"/>
-      <c r="C475" s="2"/>
+      <c r="B475" s="6"/>
+      <c r="C475" s="6"/>
     </row>
     <row r="476" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B476" s="2"/>
-      <c r="C476" s="2"/>
+      <c r="B476" s="6"/>
+      <c r="C476" s="6"/>
     </row>
     <row r="477" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B477" s="2"/>
-      <c r="C477" s="2"/>
+      <c r="B477" s="6"/>
+      <c r="C477" s="6"/>
     </row>
     <row r="478" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B478" s="2"/>
-      <c r="C478" s="2"/>
+      <c r="B478" s="6"/>
+      <c r="C478" s="6"/>
     </row>
     <row r="479" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B479" s="2"/>
-      <c r="C479" s="2"/>
+      <c r="B479" s="6"/>
+      <c r="C479" s="6"/>
     </row>
     <row r="480" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B480" s="2"/>
-      <c r="C480" s="2"/>
+      <c r="B480" s="6"/>
+      <c r="C480" s="6"/>
     </row>
     <row r="481" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B481" s="2"/>
-      <c r="C481" s="2"/>
+      <c r="B481" s="6"/>
+      <c r="C481" s="6"/>
     </row>
     <row r="482" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B482" s="2"/>
-      <c r="C482" s="2"/>
+      <c r="B482" s="6"/>
+      <c r="C482" s="6"/>
     </row>
     <row r="483" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B483" s="2"/>
-      <c r="C483" s="2"/>
+      <c r="B483" s="6"/>
+      <c r="C483" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A4:A11"/>
+    <mergeCell ref="D4:D11"/>
+    <mergeCell ref="F5:J10"/>
+  </mergeCells>
   <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Men,Women,Boys,Girls,Mixed"</formula1>
@@ -3099,7 +3147,7 @@
       <formula1>"Singles, Doubles"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{00000000-0002-0000-0000-000003000000}">
-      <formula1>"R32,R16,QF,SF,F,3rd &amp; 4th,5th &amp; 6th,7th &amp; 8th,CON"</formula1>
+      <formula1>"R32,R16,QF,SF,Final,3rd &amp; 4th,5th &amp; 6th,7th &amp; 8th,CON"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"U-09,U-11,U-13,U-15,U-17,U-19,U-21,Seniors"</formula1>

</xml_diff>

<commit_message>
added create thumbnail mfor singles and doubles
</commit_message>
<xml_diff>
--- a/match_details.xlsx
+++ b/match_details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\capna\Downloads\rsc_speedball\Scoreboard generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0597C44-AED6-4E5E-A3F4-DEC5754FCCBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78ED5FB7-05BE-4270-8CDD-6F38A42D0E19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31170" yWindow="435" windowWidth="21570" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="match_details" sheetId="1" r:id="rId1"/>
@@ -61,15 +61,6 @@
     <t>U-15</t>
   </si>
   <si>
-    <t>Doubles</t>
-  </si>
-  <si>
-    <t>Ipsum Lorem &amp; Lorem Ipsum</t>
-  </si>
-  <si>
-    <t>Lorem Ipsum &amp; Ipsum Lorem</t>
-  </si>
-  <si>
     <t>for player_1 &amp; player_2: if event is singles [format: Lorem Ipsum] else if event is doubles [format: Lorem Ipsum &amp; Ipsum Lorem]</t>
   </si>
   <si>
@@ -109,6 +100,15 @@
   </si>
   <si>
     <t>Consolation</t>
+  </si>
+  <si>
+    <t>Nader Safa &amp; Hazem Yasser</t>
+  </si>
+  <si>
+    <t>Mohamed Nagah &amp; Omar Nagah</t>
+  </si>
+  <si>
+    <t>Doubles</t>
   </si>
 </sst>
 </file>
@@ -655,14 +655,14 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1030,7 +1030,7 @@
   <dimension ref="A1:K483"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="118" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1087,47 +1087,47 @@
         <v>44653</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B3" s="8">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>17</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B3" s="10">
-        <v>0</v>
-      </c>
-      <c r="C3" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>20</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
@@ -1135,111 +1135,111 @@
       <c r="C4" s="4">
         <v>0</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>16</v>
+      <c r="D4" s="9" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="4">
         <v>0</v>
       </c>
       <c r="C5" s="4">
         <v>0</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="F5" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="F5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="4">
         <v>0</v>
       </c>
       <c r="C6" s="4">
         <v>0</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="4">
         <v>0</v>
       </c>
       <c r="C7" s="4">
         <v>0</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="4">
         <v>0</v>
       </c>
       <c r="C8" s="4">
         <v>0</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="4">
         <v>0</v>
       </c>
       <c r="C9" s="4">
         <v>0</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="4">
         <v>0</v>
       </c>
       <c r="C10" s="4">
         <v>0</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="4">
         <v>0</v>
       </c>
       <c r="C11" s="4">
         <v>0</v>
       </c>
-      <c r="D11" s="8"/>
+      <c r="D11" s="9"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12" s="4">

</xml_diff>